<commit_message>
Laba_2 code is ready.
</commit_message>
<xml_diff>
--- a/laba_2/unique_lines.xlsx
+++ b/laba_2/unique_lines.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,7 +483,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -523,7 +523,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -563,7 +563,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -603,7 +603,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -643,7 +643,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -683,7 +683,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -723,7 +723,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -763,7 +763,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -803,7 +803,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -843,7 +843,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -883,7 +883,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -898,21 +898,21 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Mastercard</t>
+          <t>Visa</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>(50, 100)</t>
+          <t>(5, 50)</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>от 5000 до 50000</t>
+          <t>меньше 5000</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>2</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13">
@@ -923,7 +923,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -943,7 +943,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>(5, 50)</t>
+          <t>(50, 100)</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -952,23 +952,23 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>90</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Косметики и мед.товаров</t>
+          <t>Одежды</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Косметика и медицина</t>
+          <t>Одежда,обувь и аксессуары</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -978,7 +978,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Visa</t>
+          <t>Mastercard</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -988,27 +988,27 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>от 5000 до 50000</t>
+          <t>меньше 5000</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>3</v>
+        <v>2888</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Косметики и мед.товаров</t>
+          <t>Одежды</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Косметика и медицина</t>
+          <t>Одежда,обувь и аксессуары</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1018,37 +1018,37 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Visa</t>
+          <t>Mastercard</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>(50, 100)</t>
+          <t>(5, 50)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>меньше 5000</t>
+          <t>от 5000 до 50000</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>112</v>
+        <v>602</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Косметики и мед.товаров</t>
+          <t>Одежды</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Косметика и медицина</t>
+          <t>Одежда,обувь и аксессуары</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1058,7 +1058,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Visa</t>
+          <t>Mastercard</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1068,11 +1068,11 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>от 5000 до 50000</t>
+          <t>меньше 5000</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>5</v>
+        <v>3215</v>
       </c>
     </row>
     <row r="17">
@@ -1083,7 +1083,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1103,16 +1103,16 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>(5, 50)</t>
+          <t>(50, 100)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>меньше 5000</t>
+          <t>от 5000 до 50000</t>
         </is>
       </c>
       <c r="H17" t="n">
-        <v>2888</v>
+        <v>669</v>
       </c>
     </row>
     <row r="18">
@@ -1123,7 +1123,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1138,7 +1138,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Mastercard</t>
+          <t>Visa</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1148,11 +1148,11 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>от 5000 до 50000</t>
+          <t>меньше 5000</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>602</v>
+        <v>3597</v>
       </c>
     </row>
     <row r="19">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1178,21 +1178,21 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Mastercard</t>
+          <t>Visa</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>(50, 100)</t>
+          <t>(5, 50)</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>меньше 5000</t>
+          <t>от 5000 до 50000</t>
         </is>
       </c>
       <c r="H19" t="n">
-        <v>3215</v>
+        <v>779</v>
       </c>
     </row>
     <row r="20">
@@ -1203,7 +1203,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1218,7 +1218,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Mastercard</t>
+          <t>Visa</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1228,11 +1228,11 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>от 5000 до 50000</t>
+          <t>меньше 5000</t>
         </is>
       </c>
       <c r="H20" t="n">
-        <v>669</v>
+        <v>4052</v>
       </c>
     </row>
     <row r="21">
@@ -1243,7 +1243,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1263,42 +1263,42 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>(5, 50)</t>
+          <t>(50, 100)</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>меньше 5000</t>
+          <t>от 5000 до 50000</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>3597</v>
+        <v>791</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Одежды</t>
+          <t>Техники</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 29</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Одежда,обувь и аксессуары</t>
+          <t>Техника</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Одежда,обувь и аксессуары</t>
+          <t>Техника</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Visa</t>
+          <t>Mastercard</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1308,77 +1308,77 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>от 5000 до 50000</t>
+          <t>меньше 5000</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>779</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Одежды</t>
+          <t>Техники</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 29</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Одежда,обувь и аксессуары</t>
+          <t>Техника</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Одежда,обувь и аксессуары</t>
+          <t>Техника</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Visa</t>
+          <t>Mastercard</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>(50, 100)</t>
+          <t>(5, 50)</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>меньше 5000</t>
+          <t>от 5000 до 50000</t>
         </is>
       </c>
       <c r="H23" t="n">
-        <v>4052</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Одежды</t>
+          <t>Техники</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 29</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Одежда,обувь и аксессуары</t>
+          <t>Техника</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Одежда,обувь и аксессуары</t>
+          <t>Техника</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Visa</t>
+          <t>Mastercard</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>от 5000 до 50000</t>
+          <t>меньше 5000</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>791</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25">
@@ -1403,7 +1403,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>'5,29.</t>
+          <t>59, 29</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1423,16 +1423,16 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>(5, 50)</t>
+          <t>(50, 100)</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>меньше 5000</t>
+          <t>от 5000 до 50000</t>
         </is>
       </c>
       <c r="H25" t="n">
-        <v>72</v>
+        <v>301</v>
       </c>
     </row>
     <row r="26">
@@ -1443,7 +1443,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>'5,29.</t>
+          <t>59, 29</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1458,7 +1458,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Mastercard</t>
+          <t>Visa</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1468,11 +1468,11 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>от 5000 до 50000</t>
+          <t>меньше 5000</t>
         </is>
       </c>
       <c r="H26" t="n">
-        <v>281</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27">
@@ -1483,7 +1483,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>'5,29.</t>
+          <t>59, 29</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1498,21 +1498,21 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Mastercard</t>
+          <t>Visa</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>(50, 100)</t>
+          <t>(5, 50)</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>меньше 5000</t>
+          <t>от 5000 до 50000</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>96</v>
+        <v>349</v>
       </c>
     </row>
     <row r="28">
@@ -1523,7 +1523,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>'5,29.</t>
+          <t>59, 29</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Mastercard</t>
+          <t>Visa</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1548,11 +1548,11 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>от 5000 до 50000</t>
+          <t>меньше 5000</t>
         </is>
       </c>
       <c r="H28" t="n">
-        <v>301</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29">
@@ -1563,7 +1563,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>'5,29.</t>
+          <t>59, 29</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1583,16 +1583,16 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>(5, 50)</t>
+          <t>(50, 100)</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>меньше 5000</t>
+          <t>от 5000 до 50000</t>
         </is>
       </c>
       <c r="H29" t="n">
-        <v>87</v>
+        <v>368</v>
       </c>
     </row>
     <row r="30">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>'5,29.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1618,7 +1618,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Visa</t>
+          <t>Mastercard</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1628,11 +1628,11 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>от 5000 до 50000</t>
+          <t>меньше 5000</t>
         </is>
       </c>
       <c r="H30" t="n">
-        <v>349</v>
+        <v>638</v>
       </c>
     </row>
     <row r="31">
@@ -1643,7 +1643,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>'5,29.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1658,21 +1658,21 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Visa</t>
+          <t>Mastercard</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>(50, 100)</t>
+          <t>(5, 50)</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>меньше 5000</t>
+          <t>от 5000 до 50000</t>
         </is>
       </c>
       <c r="H31" t="n">
-        <v>96</v>
+        <v>2182</v>
       </c>
     </row>
     <row r="32">
@@ -1683,7 +1683,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>'5,29.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1698,7 +1698,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Visa</t>
+          <t>Mastercard</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1708,11 +1708,11 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>от 5000 до 50000</t>
+          <t>меньше 5000</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>368</v>
+        <v>686</v>
       </c>
     </row>
     <row r="33">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1743,16 +1743,16 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>(5, 50)</t>
+          <t>(50, 100)</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>меньше 5000</t>
+          <t>от 5000 до 50000</t>
         </is>
       </c>
       <c r="H33" t="n">
-        <v>638</v>
+        <v>2447</v>
       </c>
     </row>
     <row r="34">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1778,7 +1778,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Mastercard</t>
+          <t>Visa</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>от 5000 до 50000</t>
+          <t>меньше 5000</t>
         </is>
       </c>
       <c r="H34" t="n">
-        <v>2182</v>
+        <v>853</v>
       </c>
     </row>
     <row r="35">
@@ -1803,7 +1803,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1818,21 +1818,21 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Mastercard</t>
+          <t>Visa</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>(50, 100)</t>
+          <t>(5, 50)</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>меньше 5000</t>
+          <t>от 5000 до 50000</t>
         </is>
       </c>
       <c r="H35" t="n">
-        <v>686</v>
+        <v>2665</v>
       </c>
     </row>
     <row r="36">
@@ -1843,7 +1843,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1858,7 +1858,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Mastercard</t>
+          <t>Visa</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1868,11 +1868,11 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>от 5000 до 50000</t>
+          <t>меньше 5000</t>
         </is>
       </c>
       <c r="H36" t="n">
-        <v>2447</v>
+        <v>901</v>
       </c>
     </row>
     <row r="37">
@@ -1883,7 +1883,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>59, 30</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1903,16 +1903,16 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>(5, 50)</t>
+          <t>(50, 100)</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>меньше 5000</t>
+          <t>от 5000 до 50000</t>
         </is>
       </c>
       <c r="H37" t="n">
-        <v>853</v>
+        <v>2950</v>
       </c>
     </row>
     <row r="38">
@@ -1923,7 +1923,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>60, 30</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Visa</t>
+          <t>Mastercard</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1948,11 +1948,11 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>от 5000 до 50000</t>
+          <t>меньше 5000</t>
         </is>
       </c>
       <c r="H38" t="n">
-        <v>2665</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>60, 30</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1978,21 +1978,21 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Visa</t>
+          <t>Mastercard</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>(50, 100)</t>
+          <t>(5, 50)</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>меньше 5000</t>
+          <t>от 5000 до 50000</t>
         </is>
       </c>
       <c r="H39" t="n">
-        <v>901</v>
+        <v>266</v>
       </c>
     </row>
     <row r="40">
@@ -2003,7 +2003,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>'5,30.</t>
+          <t>60, 30</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2018,7 +2018,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Visa</t>
+          <t>Mastercard</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2028,11 +2028,11 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>от 5000 до 50000</t>
+          <t>меньше 5000</t>
         </is>
       </c>
       <c r="H40" t="n">
-        <v>2950</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41">
@@ -2043,7 +2043,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>'6,30.</t>
+          <t>60, 30</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2063,16 +2063,16 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>(5, 50)</t>
+          <t>(50, 100)</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>меньше 5000</t>
+          <t>от 5000 до 50000</t>
         </is>
       </c>
       <c r="H41" t="n">
-        <v>94</v>
+        <v>312</v>
       </c>
     </row>
     <row r="42">
@@ -2083,7 +2083,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>'6,30.</t>
+          <t>60, 30</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2098,7 +2098,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Mastercard</t>
+          <t>Visa</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2108,11 +2108,11 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>от 5000 до 50000</t>
+          <t>меньше 5000</t>
         </is>
       </c>
       <c r="H42" t="n">
-        <v>266</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43">
@@ -2123,7 +2123,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>'6,30.</t>
+          <t>60, 30</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2138,21 +2138,21 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Mastercard</t>
+          <t>Visa</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>(50, 100)</t>
+          <t>(5, 50)</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>меньше 5000</t>
+          <t>от 5000 до 50000</t>
         </is>
       </c>
       <c r="H43" t="n">
-        <v>86</v>
+        <v>341</v>
       </c>
     </row>
     <row r="44">
@@ -2163,7 +2163,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>'6,30.</t>
+          <t>60, 30</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2178,7 +2178,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Mastercard</t>
+          <t>Visa</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2188,11 +2188,11 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>от 5000 до 50000</t>
+          <t>меньше 5000</t>
         </is>
       </c>
       <c r="H44" t="n">
-        <v>312</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45">
@@ -2203,7 +2203,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>'6,30.</t>
+          <t>60, 30</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2223,135 +2223,15 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>(5, 50)</t>
+          <t>(50, 100)</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>меньше 5000</t>
+          <t>от 5000 до 50000</t>
         </is>
       </c>
       <c r="H45" t="n">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>Техники</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>'6,30.</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Техника</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Техника</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>Visa</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>(5, 50)</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>от 5000 до 50000</t>
-        </is>
-      </c>
-      <c r="H46" t="n">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>Техники</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>'6,30.</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Техника</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>Техника</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>Visa</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>(50, 100)</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>меньше 5000</t>
-        </is>
-      </c>
-      <c r="H47" t="n">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>Техники</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>'6,30.</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Техника</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Техника</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>Visa</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>(50, 100)</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>от 5000 до 50000</t>
-        </is>
-      </c>
-      <c r="H48" t="n">
         <v>366</v>
       </c>
     </row>

</xml_diff>